<commit_message>
minor algo notation fix
</commit_message>
<xml_diff>
--- a/examples.xlsx
+++ b/examples.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="168">
   <si>
     <t xml:space="preserve">Example</t>
   </si>
@@ -56,7 +56,7 @@
 turn based</t>
   </si>
   <si>
-    <t xml:space="preserve">alpha_zero</t>
+    <t xml:space="preserve">alpha_zero.alpha_zero</t>
   </si>
   <si>
     <t xml:space="preserve">benchmark_games.py</t>
@@ -546,9 +546,6 @@
   </si>
   <si>
     <t xml:space="preserve">only game 'tic_tac_toe'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alpha_zero.alpha_zero</t>
   </si>
   <si>
     <t xml:space="preserve">tic_tac_toe_dqn_vs_tabular.py</t>
@@ -593,6 +590,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -614,12 +612,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -712,17 +712,17 @@
   <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C67" activeCellId="0" sqref="C67"/>
+      <selection pane="bottomLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.44"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1635,12 +1635,12 @@
         <v>158</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>159</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>13</v>
@@ -1652,12 +1652,12 @@
         <v>158</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>13</v>
@@ -1669,12 +1669,12 @@
         <v>158</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>13</v>
@@ -1686,12 +1686,12 @@
         <v>33</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>8</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>13</v>
@@ -1720,7 +1720,7 @@
         <v>158</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modded some examples to work
</commit_message>
<xml_diff>
--- a/examples.xlsx
+++ b/examples.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="167">
   <si>
     <t xml:space="preserve">Example</t>
   </si>
@@ -491,9 +491,6 @@
   </si>
   <si>
     <t xml:space="preserve">rl_example.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">actions &gt; 2</t>
   </si>
   <si>
     <t xml:space="preserve">rl_main_loop.py</t>
@@ -712,9 +709,9 @@
   <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1536,43 +1533,43 @@
         <v>142</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>143</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D57" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="0" t="s">
         <v>145</v>
-      </c>
-      <c r="E57" s="0" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>15</v>
@@ -1584,12 +1581,12 @@
         <v>22</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>15</v>
@@ -1598,15 +1595,15 @@
         <v>9</v>
       </c>
       <c r="D60" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>15</v>
@@ -1615,24 +1612,24 @@
         <v>9</v>
       </c>
       <c r="D61" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>158</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>11</v>
@@ -1640,41 +1637,41 @@
     </row>
     <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>13</v>
@@ -1686,12 +1683,12 @@
         <v>33</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>8</v>
@@ -1708,19 +1705,19 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E67" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>